<commit_message>
Added new entries to Attendance
</commit_message>
<xml_diff>
--- a/Documentation/Attendance.xlsx
+++ b/Documentation/Attendance.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28526"/>
-  <workbookPr defaultThemeVersion="202300"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11008"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\troll\!Coding\School\FontysRelated\Year1\Semester2\Group\Documentation\Github\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/dustinveerdonk/Downloads/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{10FEBCBD-B8A8-4ADB-B181-A15F25A5AD28}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9397F455-E274-614E-B360-798B8F5DC3AB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="30936" windowHeight="18696" xr2:uid="{02D3045F-E3D0-49C2-806F-2E2961CB537A}"/>
+    <workbookView xWindow="0" yWindow="740" windowWidth="17160" windowHeight="21600" xr2:uid="{02D3045F-E3D0-49C2-806F-2E2961CB537A}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -27,7 +27,6 @@
         <xcalcf:feature name="microsoft.com:FV"/>
         <xcalcf:feature name="microsoft.com:CNMTM"/>
         <xcalcf:feature name="microsoft.com:LET_WF"/>
-        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
         <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
       </xcalcf:calcFeatures>
     </ext>
@@ -36,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="13">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="42" uniqueCount="18">
   <si>
     <t>Tom</t>
   </si>
@@ -75,6 +74,21 @@
   </si>
   <si>
     <t>Afwezig</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Aanwezig - </t>
+  </si>
+  <si>
+    <t>Aanwezig - Niew lijst toevoegen</t>
+  </si>
+  <si>
+    <t>Aanwezig - Onduidelijk</t>
+  </si>
+  <si>
+    <t>Aanwezig - Product aan lijst toevoegen</t>
+  </si>
+  <si>
+    <t>Aanwezig - UI van pagina maken</t>
   </si>
 </sst>
 </file>
@@ -450,23 +464,24 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CC82EAEF-05B4-4689-8441-0C3B9F7DFDCE}">
-  <dimension ref="A1:G3"/>
+  <dimension ref="A1:G7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F9" sqref="F9"/>
+      <selection activeCell="D12" sqref="D12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="9.44140625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="24.109375" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="25.5546875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="29" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="19.6640625" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="21.88671875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="6.6640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="19.6640625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="23.1640625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="29.1640625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="6.5" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="29.1640625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="18.1640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.2">
       <c r="B1" s="1" t="s">
         <v>0</v>
       </c>
@@ -486,7 +501,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A2" s="2">
         <v>45789</v>
       </c>
@@ -509,13 +524,16 @@
         <v>8</v>
       </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A3" s="2">
         <v>45790</v>
       </c>
       <c r="B3" t="s">
         <v>5</v>
       </c>
+      <c r="C3" t="s">
+        <v>13</v>
+      </c>
       <c r="D3" t="s">
         <v>6</v>
       </c>
@@ -527,6 +545,98 @@
       </c>
       <c r="G3" t="s">
         <v>8</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A4" s="2">
+        <v>45796</v>
+      </c>
+      <c r="B4" t="s">
+        <v>5</v>
+      </c>
+      <c r="C4" t="s">
+        <v>13</v>
+      </c>
+      <c r="D4" t="s">
+        <v>14</v>
+      </c>
+      <c r="E4" t="s">
+        <v>12</v>
+      </c>
+      <c r="F4" t="s">
+        <v>10</v>
+      </c>
+      <c r="G4" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A5" s="2">
+        <v>45797</v>
+      </c>
+      <c r="B5" t="s">
+        <v>5</v>
+      </c>
+      <c r="C5" t="s">
+        <v>13</v>
+      </c>
+      <c r="D5" t="s">
+        <v>14</v>
+      </c>
+      <c r="E5" t="s">
+        <v>12</v>
+      </c>
+      <c r="F5" t="s">
+        <v>10</v>
+      </c>
+      <c r="G5" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A6" s="2">
+        <v>45803</v>
+      </c>
+      <c r="B6" t="s">
+        <v>5</v>
+      </c>
+      <c r="C6" t="s">
+        <v>13</v>
+      </c>
+      <c r="D6" t="s">
+        <v>16</v>
+      </c>
+      <c r="E6" t="s">
+        <v>12</v>
+      </c>
+      <c r="F6" t="s">
+        <v>16</v>
+      </c>
+      <c r="G6" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A7" s="2">
+        <v>45804</v>
+      </c>
+      <c r="B7" t="s">
+        <v>5</v>
+      </c>
+      <c r="C7" t="s">
+        <v>13</v>
+      </c>
+      <c r="D7" t="s">
+        <v>17</v>
+      </c>
+      <c r="E7" t="s">
+        <v>12</v>
+      </c>
+      <c r="F7" t="s">
+        <v>16</v>
+      </c>
+      <c r="G7" t="s">
+        <v>12</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Added weekly process to the git. Change the git ignore again
</commit_message>
<xml_diff>
--- a/Documentation/Attendance.xlsx
+++ b/Documentation/Attendance.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/dustinveerdonk/Downloads/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/dustinveerdonk/RiderProjects/LunchList/Documentation/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9397F455-E274-614E-B360-798B8F5DC3AB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{174AB55A-1B43-E944-B0BC-AEC5B4E97178}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="740" windowWidth="17160" windowHeight="21600" xr2:uid="{02D3045F-E3D0-49C2-806F-2E2961CB537A}"/>
+    <workbookView xWindow="0" yWindow="760" windowWidth="17160" windowHeight="19860" xr2:uid="{02D3045F-E3D0-49C2-806F-2E2961CB537A}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -466,7 +466,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CC82EAEF-05B4-4689-8441-0C3B9F7DFDCE}">
   <dimension ref="A1:G7"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView tabSelected="1" zoomScale="150" workbookViewId="0">
       <selection activeCell="D12" sqref="D12"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
Added Attendace and updated Weekly Progress
</commit_message>
<xml_diff>
--- a/Documentation/Attendance.xlsx
+++ b/Documentation/Attendance.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/dustinveerdonk/RiderProjects/LunchList/Documentation/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FE5A3264-E413-624F-A365-7A43DC26808C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C21AE8A5-D4C9-FC44-94D9-FB3706FC4B96}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="760" windowWidth="17160" windowHeight="19860" xr2:uid="{02D3045F-E3D0-49C2-806F-2E2961CB537A}"/>
   </bookViews>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="42" uniqueCount="21">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="54" uniqueCount="27">
   <si>
     <t>Tom</t>
   </si>
@@ -98,6 +98,24 @@
   </si>
   <si>
     <t>Aanwezig - Groeps feedback schrijven</t>
+  </si>
+  <si>
+    <t>Aanwezig - Documentation</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Aanwezig </t>
+  </si>
+  <si>
+    <t>Aanwezig</t>
+  </si>
+  <si>
+    <t>Aanwezig - gepraat over groeps process</t>
+  </si>
+  <si>
+    <t>Aanwezig - Demo</t>
+  </si>
+  <si>
+    <t>Aanwezig - groeps process vertellen</t>
   </si>
 </sst>
 </file>
@@ -473,16 +491,16 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CC82EAEF-05B4-4689-8441-0C3B9F7DFDCE}">
-  <dimension ref="A1:G7"/>
+  <dimension ref="A1:G9"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C1" zoomScale="150" workbookViewId="0">
-      <selection activeCell="E9" sqref="E9"/>
+    <sheetView tabSelected="1" topLeftCell="D1" zoomScale="150" workbookViewId="0">
+      <selection activeCell="G14" sqref="G14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="6.6640625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="20.5" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="21.83203125" customWidth="1"/>
     <col min="3" max="3" width="29.83203125" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="30.1640625" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="6.83203125" bestFit="1" customWidth="1"/>
@@ -648,6 +666,52 @@
         <v>12</v>
       </c>
     </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A8" s="2">
+        <v>45810</v>
+      </c>
+      <c r="B8" t="s">
+        <v>21</v>
+      </c>
+      <c r="C8" t="s">
+        <v>22</v>
+      </c>
+      <c r="D8" t="s">
+        <v>23</v>
+      </c>
+      <c r="E8" t="s">
+        <v>12</v>
+      </c>
+      <c r="F8" t="s">
+        <v>24</v>
+      </c>
+      <c r="G8" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A9" s="2">
+        <v>45811</v>
+      </c>
+      <c r="B9" t="s">
+        <v>21</v>
+      </c>
+      <c r="C9" t="s">
+        <v>25</v>
+      </c>
+      <c r="D9" t="s">
+        <v>23</v>
+      </c>
+      <c r="E9" t="s">
+        <v>12</v>
+      </c>
+      <c r="F9" t="s">
+        <v>26</v>
+      </c>
+      <c r="G9" t="s">
+        <v>23</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>